<commit_message>
Refactor database operations into a databases module
</commit_message>
<xml_diff>
--- a/server_files/processedCopy.xlsx
+++ b/server_files/processedCopy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\client_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C0ADDA-16C9-412E-AE58-2C8B4D3DA0EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A080BD-59E0-4E74-BCF3-516C61F6F076}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10690" yWindow="2750" windowWidth="19200" windowHeight="7640" xr2:uid="{53D2BF35-7FCC-480B-9978-13FEE58D4D09}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53D2BF35-7FCC-480B-9978-13FEE58D4D09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4130FF-8469-4445-BDF6-5FC95641EC3C}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>